<commit_message>
additional accounts - covid 19
improving coding of additional accounts
</commit_message>
<xml_diff>
--- a/simfin/missions/historical_accounts.xlsx
+++ b/simfin/missions/historical_accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliennavaux/Documents/simfin/simfin/missions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliennavaux/Documents/simfin-dev/simfin/missions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E9FA8E-32FC-5545-AEB8-CAD4709A2856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063CA4A-D0CB-C347-9A3A-80864AF2B82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="13380" windowWidth="51200" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9100" windowWidth="51200" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
@@ -450,10 +450,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +463,7 @@
     <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,8 +521,14 @@
       <c r="S1">
         <v>2021</v>
       </c>
+      <c r="T1">
+        <v>2022</v>
+      </c>
+      <c r="U1">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -581,7 +587,7 @@
         <v>46409</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -640,7 +646,7 @@
         <v>26619</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -699,7 +705,7 @@
         <v>15391</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -758,7 +764,7 @@
         <v>3668</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -817,7 +823,7 @@
         <v>2817</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -876,7 +882,7 @@
         <v>4761</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -935,7 +941,7 @@
         <v>11156</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -992,6 +998,12 @@
       </c>
       <c r="S9" s="1">
         <v>11920</v>
+      </c>
+      <c r="T9" s="1">
+        <v>4284</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>